<commit_message>
New experiment and methodology
Modified methodology for IP table and create a new experience for MLab measure.
</commit_message>
<xml_diff>
--- a/Work/SpaceX IP List.xlsx
+++ b/Work/SpaceX IP List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philemon\Documents\ULB CyberSecurity\Master Thesis\master-thesis\Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B294D5-1FDF-49D5-A33C-0A1654F4F250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92A1F39A-4D90-4387-9C10-435595EDEAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD9C249C-8872-4522-8D64-8CF6F167022A}"/>
+    <workbookView xWindow="-10635" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{CD9C249C-8872-4522-8D64-8CF6F167022A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -912,6 +912,9 @@
     <t>STRLNK-POP-FRNTDEU1-POOL0-V4</t>
   </si>
   <si>
+    <t>145.224.72.0/21</t>
+  </si>
+  <si>
     <t>145.224.96.0/21</t>
   </si>
   <si>
@@ -1153,9 +1156,6 @@
   </si>
   <si>
     <t>Public IP for users (13851)</t>
-  </si>
-  <si>
-    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -1902,7 +1902,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1912,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1EA4DA-015E-4BB8-838B-09D1BD25F0A6}">
   <dimension ref="C3:P138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,12 +1923,12 @@
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1968,7 +1968,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1986,7 +1986,7 @@
         <v>3</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
@@ -2014,18 +2014,18 @@
         <v>21</v>
       </c>
       <c r="N6" s="46" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="O6" s="48" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="P6" s="48" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" s="31" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>252</v>
@@ -2042,22 +2042,22 @@
       <c r="H7" s="6"/>
       <c r="K7" s="31"/>
       <c r="L7" s="26" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="M7" s="38" t="s">
         <v>21</v>
       </c>
       <c r="N7" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="P7" s="12"/>
     </row>
     <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C8" s="31" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>273</v>
@@ -2080,16 +2080,16 @@
         <v>21</v>
       </c>
       <c r="N8" s="26" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="P8" s="12"/>
     </row>
     <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C9" s="31" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>274</v>
@@ -2106,16 +2106,16 @@
       <c r="H9" s="6"/>
       <c r="K9" s="31"/>
       <c r="L9" s="26" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M9" s="38" t="s">
         <v>21</v>
       </c>
       <c r="N9" s="26" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="P9" s="12"/>
     </row>
@@ -2142,10 +2142,10 @@
         <v>21</v>
       </c>
       <c r="N10" s="26" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="P10" s="12"/>
     </row>
@@ -2168,19 +2168,19 @@
       <c r="H11" s="7"/>
       <c r="K11" s="31"/>
       <c r="L11" s="26" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="M11" s="49" t="s">
         <v>21</v>
       </c>
       <c r="N11" s="19" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.25">
@@ -2206,10 +2206,10 @@
         <v>21</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="P12" s="12"/>
     </row>
@@ -2220,26 +2220,26 @@
       </c>
       <c r="E13" s="41"/>
       <c r="F13" s="22" t="s">
-        <v>366</v>
+        <v>285</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>284</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K13" s="31"/>
       <c r="L13" s="26" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M13" s="38" t="s">
         <v>21</v>
       </c>
       <c r="N13" s="26" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="P13" s="12"/>
     </row>
@@ -2250,10 +2250,10 @@
       </c>
       <c r="E14" s="41"/>
       <c r="F14" s="22" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H14" s="9"/>
       <c r="K14" s="32" t="s">
@@ -2266,24 +2266,24 @@
         <v>21</v>
       </c>
       <c r="N14" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="O14" s="11" t="s">
         <v>302</v>
-      </c>
-      <c r="O14" s="11" t="s">
-        <v>301</v>
       </c>
       <c r="P14" s="11"/>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C15" s="34"/>
       <c r="D15" s="28" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E15" s="41"/>
       <c r="F15" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>288</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>287</v>
       </c>
       <c r="H15" s="9"/>
       <c r="K15" s="32" t="s">
@@ -2296,26 +2296,26 @@
         <v>51</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="P15" s="11"/>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C16" s="34" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E16" s="41"/>
       <c r="F16" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>291</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>290</v>
       </c>
       <c r="H16" s="9"/>
       <c r="K16" s="32" t="s">
@@ -2328,10 +2328,10 @@
         <v>51</v>
       </c>
       <c r="N16" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="O16" s="11" t="s">
         <v>322</v>
-      </c>
-      <c r="O16" s="11" t="s">
-        <v>321</v>
       </c>
       <c r="P16" s="11"/>
     </row>
@@ -2362,10 +2362,10 @@
         <v>51</v>
       </c>
       <c r="N17" s="24" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="P17" s="11"/>
     </row>
@@ -2392,10 +2392,10 @@
         <v>51</v>
       </c>
       <c r="N18" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="O18" s="11" t="s">
         <v>326</v>
-      </c>
-      <c r="O18" s="11" t="s">
-        <v>325</v>
       </c>
       <c r="P18" s="11"/>
     </row>
@@ -2424,10 +2424,10 @@
         <v>51</v>
       </c>
       <c r="N19" s="24" t="s">
+        <v>329</v>
+      </c>
+      <c r="O19" s="11" t="s">
         <v>328</v>
-      </c>
-      <c r="O19" s="11" t="s">
-        <v>327</v>
       </c>
       <c r="P19" s="11"/>
     </row>
@@ -2456,10 +2456,10 @@
         <v>51</v>
       </c>
       <c r="N20" s="24" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="O20" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="P20" s="11"/>
     </row>
@@ -2488,10 +2488,10 @@
         <v>51</v>
       </c>
       <c r="N21" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="O21" s="11" t="s">
         <v>334</v>
-      </c>
-      <c r="O21" s="11" t="s">
-        <v>333</v>
       </c>
       <c r="P21" s="11"/>
     </row>
@@ -2522,10 +2522,10 @@
         <v>51</v>
       </c>
       <c r="N22" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="O22" s="11" t="s">
         <v>336</v>
-      </c>
-      <c r="O22" s="11" t="s">
-        <v>335</v>
       </c>
       <c r="P22" s="11"/>
     </row>
@@ -2554,10 +2554,10 @@
         <v>51</v>
       </c>
       <c r="N23" s="24" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="O23" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="P23" s="11"/>
     </row>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="H24" s="11"/>
       <c r="K24" s="32" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L24" s="24" t="s">
         <v>50</v>
@@ -2588,13 +2588,13 @@
         <v>51</v>
       </c>
       <c r="N24" s="24" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="O24" s="11" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
@@ -2612,7 +2612,7 @@
         <v>24</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="K25" s="31"/>
       <c r="L25" s="26" t="s">
@@ -2622,10 +2622,10 @@
         <v>51</v>
       </c>
       <c r="N25" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="O25" s="12" t="s">
         <v>343</v>
-      </c>
-      <c r="O25" s="12" t="s">
-        <v>342</v>
       </c>
       <c r="P25" s="12"/>
     </row>
@@ -2644,22 +2644,22 @@
         <v>23</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="K26" s="32" t="s">
         <v>232</v>
       </c>
       <c r="L26" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="M26" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="N26" s="24" t="s">
+        <v>347</v>
+      </c>
+      <c r="O26" s="11" t="s">
         <v>345</v>
-      </c>
-      <c r="M26" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="N26" s="24" t="s">
-        <v>346</v>
-      </c>
-      <c r="O26" s="11" t="s">
-        <v>344</v>
       </c>
       <c r="P26" s="11"/>
     </row>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="H27" s="12"/>
       <c r="K27" s="32" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L27" s="24" t="s">
         <v>50</v>
@@ -2688,10 +2688,10 @@
         <v>51</v>
       </c>
       <c r="N27" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="O27" s="11" t="s">
         <v>348</v>
-      </c>
-      <c r="O27" s="11" t="s">
-        <v>347</v>
       </c>
       <c r="P27" s="11"/>
     </row>
@@ -2716,13 +2716,13 @@
         <v>169</v>
       </c>
       <c r="N28" s="56" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="O28" s="58" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="P28" s="58" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="29" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2732,13 +2732,13 @@
       </c>
       <c r="E29" s="41"/>
       <c r="F29" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="G29" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="G29" s="14" t="s">
-        <v>293</v>
-      </c>
       <c r="H29" s="14" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="K29" s="51" t="s">
         <v>100</v>
@@ -2750,26 +2750,26 @@
         <v>102</v>
       </c>
       <c r="N29" s="52" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="O29" s="54" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="P29" s="54"/>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="34" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E30" s="41"/>
       <c r="F30" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="G30" s="14" t="s">
         <v>296</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>295</v>
       </c>
       <c r="H30" s="14"/>
     </row>
@@ -2838,7 +2838,7 @@
         <v>264</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
         <v>39</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
@@ -3360,7 +3360,7 @@
         <v>158</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
@@ -3496,7 +3496,7 @@
         <v>121</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.25">
@@ -4208,7 +4208,7 @@
         <v>260</v>
       </c>
       <c r="H115" s="10" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.25">

</xml_diff>